<commit_message>
Update Task 3A - Sprint Logs.xlsx
</commit_message>
<xml_diff>
--- a/All Tasks/Task 3A - Sprint Logs.xlsx
+++ b/All Tasks/Task 3A - Sprint Logs.xlsx
@@ -321,7 +321,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t>4th Sprint Burndown Chart</a:t>
+              <a:t>5th Sprint Burndown Chart</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -677,25 +677,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.5</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2</c:v>
@@ -1895,13 +1895,13 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:C30"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="85" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
   </cols>
@@ -2185,8 +2185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,7 +2233,7 @@
         <v>24</v>
       </c>
       <c r="G3">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2254,7 +2254,7 @@
         <v>21.6</v>
       </c>
       <c r="G4">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2276,7 +2276,7 @@
         <v>19.2</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2298,7 +2298,7 @@
         <v>16.8</v>
       </c>
       <c r="G6">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2321,7 +2321,7 @@
         <v>14.4</v>
       </c>
       <c r="G7">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2344,7 +2344,7 @@
         <v>12</v>
       </c>
       <c r="G8">
-        <v>7.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2367,7 +2367,7 @@
         <v>9.6000000000000014</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="G14">
         <f>Actual</f>
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="G15">
         <f>(Actual - Total_Effort)</f>
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>